<commit_message>
Support raffle claiming by date range
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/raffleTicketClaim.xlsx
+++ b/src/main/resources/excel/raffleTicketClaim.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJ\git\magic\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033DE3C7-7453-49B2-BDEA-5C8923F3746C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE87932-5DDF-4E38-8A56-E7C90F85E605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -372,29 +372,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -402,16 +403,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>